<commit_message>
Delete contact, add in kind gift, add git
</commit_message>
<xml_diff>
--- a/Framework/TestData/Data.xlsx
+++ b/Framework/TestData/Data.xlsx
@@ -4,12 +4,18 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="164011"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12648" activeTab="2"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12648" firstSheet="3" activeTab="8"/>
   </bookViews>
   <sheets>
     <sheet name="Login" sheetId="1" r:id="rId1"/>
     <sheet name="Individual" sheetId="2" r:id="rId2"/>
     <sheet name="AddIndividualFullDetails" sheetId="3" r:id="rId3"/>
+    <sheet name="Organization" sheetId="4" r:id="rId4"/>
+    <sheet name="OrganizationFullDetails" sheetId="5" r:id="rId5"/>
+    <sheet name="DeleteContact" sheetId="6" r:id="rId6"/>
+    <sheet name="AddInKindGift" sheetId="7" r:id="rId7"/>
+    <sheet name="AddGift" sheetId="8" r:id="rId8"/>
+    <sheet name="Appeal" sheetId="9" r:id="rId9"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -21,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="77" uniqueCount="56">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="175" uniqueCount="117">
   <si>
     <t>navlu</t>
   </si>
@@ -189,6 +195,189 @@
   </si>
   <si>
     <t>ab2122112c@gmail.com</t>
+  </si>
+  <si>
+    <t>Organization Name</t>
+  </si>
+  <si>
+    <t>ID</t>
+  </si>
+  <si>
+    <t>URL</t>
+  </si>
+  <si>
+    <t>No of Employee</t>
+  </si>
+  <si>
+    <t>Address line 1</t>
+  </si>
+  <si>
+    <t>Address line 2</t>
+  </si>
+  <si>
+    <t>County</t>
+  </si>
+  <si>
+    <t>www.testorg.com</t>
+  </si>
+  <si>
+    <t>ABC address</t>
+  </si>
+  <si>
+    <t>address line 2</t>
+  </si>
+  <si>
+    <t>Sonoma</t>
+  </si>
+  <si>
+    <t>Cotati</t>
+  </si>
+  <si>
+    <t>TestOrg1234</t>
+  </si>
+  <si>
+    <t>info@testorg123.com</t>
+  </si>
+  <si>
+    <t>PrimaryNPContact</t>
+  </si>
+  <si>
+    <t>OrganizationName</t>
+  </si>
+  <si>
+    <t>Number of Employee</t>
+  </si>
+  <si>
+    <t>Website</t>
+  </si>
+  <si>
+    <t>Year Founded</t>
+  </si>
+  <si>
+    <t>PrimaryContact</t>
+  </si>
+  <si>
+    <t>Job Title</t>
+  </si>
+  <si>
+    <t>Contact For</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Address Line1 </t>
+  </si>
+  <si>
+    <t>PhoneCall</t>
+  </si>
+  <si>
+    <t>Crucial Information</t>
+  </si>
+  <si>
+    <t>Google</t>
+  </si>
+  <si>
+    <t>www.google.com</t>
+  </si>
+  <si>
+    <t>Manager</t>
+  </si>
+  <si>
+    <t>Sales and Marketing</t>
+  </si>
+  <si>
+    <t>Mr. Chait</t>
+  </si>
+  <si>
+    <t>Google Online</t>
+  </si>
+  <si>
+    <t>Google 2</t>
+  </si>
+  <si>
+    <t>google@test.com</t>
+  </si>
+  <si>
+    <t>Google is great.</t>
+  </si>
+  <si>
+    <t>ContactName</t>
+  </si>
+  <si>
+    <t>Contact Last name</t>
+  </si>
+  <si>
+    <t>Fund Name</t>
+  </si>
+  <si>
+    <t>Annual</t>
+  </si>
+  <si>
+    <t>Source</t>
+  </si>
+  <si>
+    <t>10 - Mail</t>
+  </si>
+  <si>
+    <t>Value</t>
+  </si>
+  <si>
+    <t>Description</t>
+  </si>
+  <si>
+    <t>This is automation in-kind</t>
+  </si>
+  <si>
+    <t>Gift Memo</t>
+  </si>
+  <si>
+    <t>Memo testing</t>
+  </si>
+  <si>
+    <t>DonorName</t>
+  </si>
+  <si>
+    <t>FundName</t>
+  </si>
+  <si>
+    <t>Program</t>
+  </si>
+  <si>
+    <t>Campaign</t>
+  </si>
+  <si>
+    <t>Payment Mode</t>
+  </si>
+  <si>
+    <t>Payment Date</t>
+  </si>
+  <si>
+    <t>Reference</t>
+  </si>
+  <si>
+    <t>Amount</t>
+  </si>
+  <si>
+    <t>Education</t>
+  </si>
+  <si>
+    <t>Cash</t>
+  </si>
+  <si>
+    <t>05/15/2021</t>
+  </si>
+  <si>
+    <t>Xyz123</t>
+  </si>
+  <si>
+    <t>Annual Fund</t>
+  </si>
+  <si>
+    <t>//label[@for='r-ask1']</t>
+  </si>
+  <si>
+    <t>Donor Name</t>
+  </si>
+  <si>
+    <t>Fundname</t>
   </si>
 </sst>
 </file>
@@ -559,7 +748,7 @@
   <dimension ref="A1:B2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A3" sqref="A3"/>
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -589,8 +778,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:Y3"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="I1" workbookViewId="0">
-      <selection activeCell="W2" sqref="W2"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -846,4 +1035,556 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" verticalDpi="0" r:id="rId3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:M3"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A9" sqref="A9"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="16.77734375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="16" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="11" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="12" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="14.21875" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="11.5546875" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A1" t="s">
+        <v>56</v>
+      </c>
+      <c r="B1" t="s">
+        <v>39</v>
+      </c>
+      <c r="C1" t="s">
+        <v>41</v>
+      </c>
+      <c r="D1" t="s">
+        <v>57</v>
+      </c>
+      <c r="E1" t="s">
+        <v>58</v>
+      </c>
+      <c r="F1" t="s">
+        <v>59</v>
+      </c>
+      <c r="G1" t="s">
+        <v>60</v>
+      </c>
+      <c r="H1" t="s">
+        <v>61</v>
+      </c>
+      <c r="I1" t="s">
+        <v>19</v>
+      </c>
+      <c r="J1" t="s">
+        <v>32</v>
+      </c>
+      <c r="K1" t="s">
+        <v>62</v>
+      </c>
+      <c r="L1" t="s">
+        <v>20</v>
+      </c>
+      <c r="M1" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="2" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A2" t="s">
+        <v>68</v>
+      </c>
+      <c r="B2" s="5" t="s">
+        <v>69</v>
+      </c>
+      <c r="C2">
+        <v>7871234551</v>
+      </c>
+      <c r="D2">
+        <v>121312312321</v>
+      </c>
+      <c r="E2" s="5" t="s">
+        <v>63</v>
+      </c>
+      <c r="F2">
+        <v>20</v>
+      </c>
+      <c r="G2" t="s">
+        <v>64</v>
+      </c>
+      <c r="H2" t="s">
+        <v>65</v>
+      </c>
+      <c r="I2">
+        <v>94928</v>
+      </c>
+      <c r="J2" t="s">
+        <v>67</v>
+      </c>
+      <c r="K2" t="s">
+        <v>66</v>
+      </c>
+      <c r="L2" t="s">
+        <v>34</v>
+      </c>
+      <c r="M2" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="3" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A3">
+        <v>0</v>
+      </c>
+      <c r="B3">
+        <v>1</v>
+      </c>
+      <c r="C3">
+        <v>2</v>
+      </c>
+      <c r="D3">
+        <v>3</v>
+      </c>
+      <c r="E3">
+        <v>4</v>
+      </c>
+      <c r="F3">
+        <v>5</v>
+      </c>
+      <c r="G3">
+        <v>6</v>
+      </c>
+      <c r="H3">
+        <v>7</v>
+      </c>
+      <c r="I3">
+        <v>8</v>
+      </c>
+      <c r="J3">
+        <v>9</v>
+      </c>
+      <c r="K3">
+        <v>10</v>
+      </c>
+      <c r="L3">
+        <v>11</v>
+      </c>
+      <c r="M3">
+        <v>12</v>
+      </c>
+    </row>
+  </sheetData>
+  <hyperlinks>
+    <hyperlink ref="B2" r:id="rId1"/>
+    <hyperlink ref="E2" r:id="rId2"/>
+  </hyperlinks>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:T2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E8" sqref="E8"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="16.109375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="16.33203125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="18.44140625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="12.109375" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="13.77734375" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="10.5546875" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="15.44140625" bestFit="1" customWidth="1"/>
+    <col min="11" max="12" width="12.5546875" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="11" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:20" x14ac:dyDescent="0.3">
+      <c r="A1" t="s">
+        <v>70</v>
+      </c>
+      <c r="B1" t="s">
+        <v>71</v>
+      </c>
+      <c r="C1" t="s">
+        <v>72</v>
+      </c>
+      <c r="D1" t="s">
+        <v>73</v>
+      </c>
+      <c r="E1" t="s">
+        <v>74</v>
+      </c>
+      <c r="F1" t="s">
+        <v>57</v>
+      </c>
+      <c r="G1" t="s">
+        <v>75</v>
+      </c>
+      <c r="H1" t="s">
+        <v>76</v>
+      </c>
+      <c r="I1" t="s">
+        <v>77</v>
+      </c>
+      <c r="J1" t="s">
+        <v>15</v>
+      </c>
+      <c r="K1" t="s">
+        <v>78</v>
+      </c>
+      <c r="L1" t="s">
+        <v>18</v>
+      </c>
+      <c r="M1" t="s">
+        <v>19</v>
+      </c>
+      <c r="N1" t="s">
+        <v>32</v>
+      </c>
+      <c r="O1" t="s">
+        <v>39</v>
+      </c>
+      <c r="P1" t="s">
+        <v>41</v>
+      </c>
+      <c r="Q1" t="s">
+        <v>79</v>
+      </c>
+      <c r="R1" t="s">
+        <v>43</v>
+      </c>
+      <c r="S1" t="s">
+        <v>44</v>
+      </c>
+      <c r="T1" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="2" spans="1:20" x14ac:dyDescent="0.3">
+      <c r="A2" t="s">
+        <v>4</v>
+      </c>
+      <c r="B2" t="s">
+        <v>81</v>
+      </c>
+      <c r="C2">
+        <v>200</v>
+      </c>
+      <c r="D2" s="5" t="s">
+        <v>82</v>
+      </c>
+      <c r="E2">
+        <v>1992</v>
+      </c>
+      <c r="F2">
+        <v>20210622</v>
+      </c>
+      <c r="G2" t="s">
+        <v>4</v>
+      </c>
+      <c r="H2" t="s">
+        <v>83</v>
+      </c>
+      <c r="I2" t="s">
+        <v>84</v>
+      </c>
+      <c r="J2" t="s">
+        <v>85</v>
+      </c>
+      <c r="K2" t="s">
+        <v>86</v>
+      </c>
+      <c r="L2" t="s">
+        <v>87</v>
+      </c>
+      <c r="M2">
+        <v>94928</v>
+      </c>
+      <c r="N2" t="s">
+        <v>67</v>
+      </c>
+      <c r="O2" s="5" t="s">
+        <v>88</v>
+      </c>
+      <c r="P2">
+        <v>8901231234</v>
+      </c>
+      <c r="Q2" t="s">
+        <v>38</v>
+      </c>
+      <c r="R2" t="s">
+        <v>45</v>
+      </c>
+      <c r="S2" t="s">
+        <v>38</v>
+      </c>
+      <c r="T2" t="s">
+        <v>89</v>
+      </c>
+    </row>
+  </sheetData>
+  <hyperlinks>
+    <hyperlink ref="D2" r:id="rId1"/>
+    <hyperlink ref="O2" r:id="rId2"/>
+  </hyperlinks>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:B2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C2" sqref="C2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="12.33203125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A1" t="s">
+        <v>90</v>
+      </c>
+      <c r="B1" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A2" t="s">
+        <v>4</v>
+      </c>
+      <c r="B2" t="s">
+        <v>5</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:F3"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C2" sqref="C2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="12.33203125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="10.21875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="22.109375" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A1" t="s">
+        <v>90</v>
+      </c>
+      <c r="B1" t="s">
+        <v>92</v>
+      </c>
+      <c r="C1" t="s">
+        <v>94</v>
+      </c>
+      <c r="D1" t="s">
+        <v>96</v>
+      </c>
+      <c r="E1" t="s">
+        <v>97</v>
+      </c>
+      <c r="F1" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A2" t="s">
+        <v>4</v>
+      </c>
+      <c r="B2" t="s">
+        <v>93</v>
+      </c>
+      <c r="C2" t="s">
+        <v>95</v>
+      </c>
+      <c r="D2">
+        <v>100</v>
+      </c>
+      <c r="E2" t="s">
+        <v>98</v>
+      </c>
+      <c r="F2" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A3">
+        <v>0</v>
+      </c>
+      <c r="B3">
+        <v>1</v>
+      </c>
+      <c r="C3">
+        <v>2</v>
+      </c>
+      <c r="D3">
+        <v>3</v>
+      </c>
+      <c r="E3">
+        <v>4</v>
+      </c>
+      <c r="F3">
+        <v>5</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:I2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C1" sqref="C1:E2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="11" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="9.77734375" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="13.44140625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="12.44140625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="19.109375" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A1" t="s">
+        <v>101</v>
+      </c>
+      <c r="B1" t="s">
+        <v>102</v>
+      </c>
+      <c r="C1" t="s">
+        <v>94</v>
+      </c>
+      <c r="D1" t="s">
+        <v>103</v>
+      </c>
+      <c r="E1" t="s">
+        <v>104</v>
+      </c>
+      <c r="F1" t="s">
+        <v>105</v>
+      </c>
+      <c r="G1" t="s">
+        <v>106</v>
+      </c>
+      <c r="H1" t="s">
+        <v>107</v>
+      </c>
+      <c r="I1" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A2" t="s">
+        <v>4</v>
+      </c>
+      <c r="B2" t="s">
+        <v>113</v>
+      </c>
+      <c r="C2" t="s">
+        <v>95</v>
+      </c>
+      <c r="D2" t="s">
+        <v>109</v>
+      </c>
+      <c r="E2">
+        <v>2015</v>
+      </c>
+      <c r="F2" t="s">
+        <v>110</v>
+      </c>
+      <c r="G2" t="s">
+        <v>111</v>
+      </c>
+      <c r="H2" t="s">
+        <v>112</v>
+      </c>
+      <c r="I2" t="s">
+        <v>114</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" verticalDpi="0" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:E2"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F1" sqref="F1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="11.44140625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="10.88671875" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A1" t="s">
+        <v>115</v>
+      </c>
+      <c r="B1" t="s">
+        <v>116</v>
+      </c>
+      <c r="C1" t="s">
+        <v>94</v>
+      </c>
+      <c r="D1" t="s">
+        <v>103</v>
+      </c>
+      <c r="E1" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A2" t="s">
+        <v>4</v>
+      </c>
+      <c r="B2" t="s">
+        <v>113</v>
+      </c>
+      <c r="C2" t="s">
+        <v>95</v>
+      </c>
+      <c r="D2" t="s">
+        <v>109</v>
+      </c>
+      <c r="E2">
+        <v>2015</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>